<commit_message>
Codificação da tabela de testes.
</commit_message>
<xml_diff>
--- a/CauseEffectDiagram/notes/Tabela de Testes.xlsx
+++ b/CauseEffectDiagram/notes/Tabela de Testes.xlsx
@@ -45,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,8 +92,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +114,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -384,7 +398,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -423,6 +437,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
@@ -444,19 +463,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3975100</xdr:colOff>
+      <xdr:colOff>3987800</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
+        <xdr:cNvPr id="4" name="Imagem 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -469,8 +488,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="50800" y="2374900"/>
-          <a:ext cx="7518400" cy="3098800"/>
+          <a:off x="0" y="2451100"/>
+          <a:ext cx="7581900" cy="3073400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -482,19 +501,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5041900</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>4076700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2"/>
+        <xdr:cNvPr id="6" name="Imagem 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -507,8 +526,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10922000" y="2857500"/>
-          <a:ext cx="11811000" cy="5232400"/>
+          <a:off x="7670800" y="3111500"/>
+          <a:ext cx="12153900" cy="5207000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -785,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="K13" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1136,10 +1155,10 @@
         <v>0</v>
       </c>
       <c r="Q10" s="26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R10" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" s="26"/>
       <c r="T10" s="26"/>
@@ -1216,53 +1235,53 @@
       </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.2">
-      <c r="L12" s="28">
-        <v>1</v>
-      </c>
-      <c r="M12" s="29">
-        <v>1</v>
-      </c>
-      <c r="N12" s="29">
-        <v>1</v>
-      </c>
-      <c r="O12" s="29">
-        <v>1</v>
-      </c>
-      <c r="P12" s="29">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="29">
-        <v>1</v>
-      </c>
-      <c r="R12" s="29">
-        <v>0</v>
-      </c>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29">
-        <v>1</v>
-      </c>
-      <c r="U12" s="29">
-        <v>1</v>
-      </c>
-      <c r="V12" s="29">
-        <v>1</v>
-      </c>
-      <c r="W12" s="29">
-        <v>0</v>
-      </c>
-      <c r="X12" s="29">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="30">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="30">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="30">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="31">
+      <c r="L12" s="38">
+        <v>1</v>
+      </c>
+      <c r="M12" s="39">
+        <v>1</v>
+      </c>
+      <c r="N12" s="39">
+        <v>1</v>
+      </c>
+      <c r="O12" s="39">
+        <v>1</v>
+      </c>
+      <c r="P12" s="42">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="42">
+        <v>1</v>
+      </c>
+      <c r="R12" s="39">
+        <v>0</v>
+      </c>
+      <c r="S12" s="39"/>
+      <c r="T12" s="39">
+        <v>1</v>
+      </c>
+      <c r="U12" s="39">
+        <v>1</v>
+      </c>
+      <c r="V12" s="39">
+        <v>1</v>
+      </c>
+      <c r="W12" s="39">
+        <v>0</v>
+      </c>
+      <c r="X12" s="39">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="40">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="40">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="40">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="41">
         <v>0</v>
       </c>
     </row>

</xml_diff>